<commit_message>
added final paper for peer review
</commit_message>
<xml_diff>
--- a/Assign3_DecisionTable_JustinOrtiz.xlsx
+++ b/Assign3_DecisionTable_JustinOrtiz.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Documents\Software Test &amp; QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle Bechtel\Documents\GitHub\SWE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="56">
   <si>
     <t>R1</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>R31</t>
+  </si>
+  <si>
+    <t>Decision Table</t>
   </si>
 </sst>
 </file>
@@ -548,9 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -559,7 +560,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>